<commit_message>
ToDoRist Change and Buttons
buttons and TodoRist's checked
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Git\SelectWorm\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="27975" windowHeight="12510"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>UI</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -171,14 +176,18 @@
   </si>
   <si>
     <t>result_R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>o</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,9 +226,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -230,6 +242,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -276,7 +296,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -308,9 +328,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,6 +363,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -517,39 +539,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="3" max="3" width="20.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -557,7 +579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -565,7 +587,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -573,7 +595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -581,7 +603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -589,30 +611,36 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -620,7 +648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -628,14 +656,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -643,7 +671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -651,18 +679,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -670,7 +698,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -678,7 +706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -686,7 +714,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -694,7 +722,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -702,7 +730,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>6</v>
       </c>
@@ -710,7 +738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>7</v>
       </c>
@@ -718,7 +746,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8</v>
       </c>
@@ -726,7 +754,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>9</v>
       </c>
@@ -734,18 +762,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -753,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -761,7 +789,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -769,7 +797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
@@ -777,7 +805,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>5</v>
       </c>
@@ -785,7 +813,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>6</v>
       </c>
@@ -793,7 +821,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>7</v>
       </c>
@@ -801,7 +829,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>8</v>
       </c>
@@ -809,38 +837,38 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>38</v>
       </c>
@@ -861,12 +889,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -874,12 +902,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>